<commit_message>
change style upload file
</commit_message>
<xml_diff>
--- a/client-vite/public/data/Upload/task_sample_import.xlsx
+++ b/client-vite/public/data/Upload/task_sample_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Visual_Studio_Code\WebCode\DATN\qlcv-refactor\client-vite\public\data\Upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\HustData\20232\DATN\PHAN BIEN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0999798D-C28E-43CC-99A8-03CD8819D7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D536C9BC-4E9D-42B1-9ECD-086A4684754A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3BFFA96E-425A-42BF-83B4-C61611C78456}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
   <si>
     <t>ID Công việc</t>
   </si>
@@ -65,21 +65,6 @@
     <t>Task ID</t>
   </si>
   <si>
-    <t>Task Code</t>
-  </si>
-  <si>
-    <t>Task Name</t>
-  </si>
-  <si>
-    <t>KPI In Task</t>
-  </si>
-  <si>
-    <t>Task Weight</t>
-  </si>
-  <si>
-    <t>Estimate Time</t>
-  </si>
-  <si>
     <t>Preceeding Tasks</t>
   </si>
   <si>
@@ -224,9 +209,6 @@
     <t>Kiểm thử tự động</t>
   </si>
   <si>
-    <t>assetType</t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
@@ -278,14 +260,65 @@
     <t>Phân tích, xây dựng chức năng, module</t>
   </si>
   <si>
+    <t>Thẻ công việc</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>analysis</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>NOTE: Với các trường nhiều giá trị như "Thẻ công việc", "Công việc tiền nhiệm", viết cách nhau bởi dấu ","</t>
+  </si>
+  <si>
     <t>preceedingTasks</t>
+  </si>
+  <si>
+    <t>Phòng họp</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>requireType</t>
+  </si>
+  <si>
+    <t>Task Code (*)</t>
+  </si>
+  <si>
+    <t>Task Name(*)</t>
+  </si>
+  <si>
+    <t>Tags(*)</t>
+  </si>
+  <si>
+    <t>KPI In Task(*)</t>
+  </si>
+  <si>
+    <t>Task Weight(*)</t>
+  </si>
+  <si>
+    <t>Estimate Time(*)</t>
+  </si>
+  <si>
+    <t>NOTE: Các trường thông tin bắt buộc có dấu (*)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +336,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
@@ -330,7 +370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -458,11 +498,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -485,6 +534,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -821,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9D3FDA-1816-40CE-B417-3393FB5FE0D1}">
-  <dimension ref="A1:U103"/>
+  <dimension ref="A1:W120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="83" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,29 +887,37 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="44" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="H1" s="15" t="s">
-        <v>78</v>
-      </c>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="J1" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
@@ -866,261 +929,271 @@
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
       <c r="U1" s="15"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="H2" s="2" t="s">
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="O3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" s="5" t="s">
+      <c r="S3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="H3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="H4" t="s">
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
         <v>21</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
         <v>25</v>
       </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" t="s">
-        <v>72</v>
-      </c>
-      <c r="U4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>36</v>
-      </c>
-      <c r="T5" t="s">
-        <v>73</v>
-      </c>
-      <c r="U5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" t="s">
-        <v>38</v>
-      </c>
-      <c r="P7" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="I8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" t="s">
-        <v>39</v>
-      </c>
-      <c r="O8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="I9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1131,217 +1204,249 @@
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="J10" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="14" t="s">
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="13"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="13"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="J11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="U11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="V11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="N12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L11" s="2" t="s">
+      <c r="O12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N11" s="5" t="s">
+      <c r="Q12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R12" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="O11" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="2" t="s">
+      <c r="S12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="T12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="U12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="P12" s="11" t="s">
+      <c r="V12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W12" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="3">
+        <v>76</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="3">
         <v>0.22800000000000001</v>
       </c>
-      <c r="F13" s="3">
+      <c r="H13" s="3">
         <v>7</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="10">
+      <c r="I13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="10">
         <v>2</v>
       </c>
-      <c r="J13" s="3">
+      <c r="L13" s="3">
         <v>2</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="10"/>
+      <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="R13" s="10"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="U13" s="3">
+        <v>1</v>
+      </c>
+      <c r="V13" s="3">
+        <v>2</v>
+      </c>
+      <c r="W13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="8"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1354,17 +1459,19 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="8"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1377,17 +1484,19 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="8"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1400,17 +1509,19 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="8"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="8"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1423,17 +1534,19 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="8"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="I18" s="8"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1446,17 +1559,19 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="8"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="I19" s="8"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1469,17 +1584,19 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="8"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="8"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1492,17 +1609,19 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="8"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="8"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1515,17 +1634,19 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="8"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="8"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1538,17 +1659,19 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="8"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1561,17 +1684,19 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="8"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="I24" s="8"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1584,17 +1709,19 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="8"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="8"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1607,17 +1734,19 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="8"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="8"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1630,17 +1759,19 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="8"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="8"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -1653,17 +1784,19 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="8"/>
+      <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="8"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -1676,17 +1809,19 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="8"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="I29" s="8"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -1699,17 +1834,19 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="8"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="I30" s="8"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -1722,17 +1859,19 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="8"/>
+      <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="I31" s="8"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -1745,17 +1884,19 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="8"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="8"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -1768,17 +1909,19 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="8"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="I33" s="8"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -1791,17 +1934,19 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="8"/>
+      <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
+      <c r="I34" s="8"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
@@ -1814,17 +1959,19 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="8"/>
+      <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
+      <c r="I35" s="8"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -1837,17 +1984,19 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="8"/>
+      <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
+      <c r="I36" s="8"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
@@ -1860,17 +2009,19 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="8"/>
+      <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+      <c r="I37" s="8"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -1883,17 +2034,19 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="8"/>
+      <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+      <c r="I38" s="8"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -1906,17 +2059,19 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="8"/>
+      <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
+      <c r="I39" s="8"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
@@ -1929,17 +2084,19 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="8"/>
+      <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
+      <c r="I40" s="8"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -1952,17 +2109,19 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="8"/>
+      <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="I41" s="8"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
@@ -1975,17 +2134,19 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="8"/>
+      <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
+      <c r="I42" s="8"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
@@ -1998,17 +2159,19 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="8"/>
+      <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
+      <c r="I43" s="8"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -2021,17 +2184,19 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="8"/>
+      <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
+      <c r="I44" s="8"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
@@ -2044,17 +2209,19 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="8"/>
+      <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
+      <c r="I45" s="8"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
@@ -2067,17 +2234,19 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V45" s="3"/>
+      <c r="W45" s="3"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="8"/>
+      <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+      <c r="I46" s="8"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
@@ -2090,17 +2259,19 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="8"/>
+      <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
+      <c r="I47" s="8"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -2113,17 +2284,19 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
       <c r="U47" s="3"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="8"/>
+      <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
+      <c r="I48" s="8"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
@@ -2136,17 +2309,19 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="8"/>
+      <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
+      <c r="I49" s="8"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
@@ -2159,17 +2334,19 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="8"/>
+      <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="I50" s="8"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
@@ -2182,17 +2359,19 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="8"/>
+      <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+      <c r="I51" s="8"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
@@ -2205,17 +2384,19 @@
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
       <c r="U51" s="3"/>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="8"/>
+      <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
+      <c r="I52" s="8"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
@@ -2228,17 +2409,19 @@
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="8"/>
+      <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
+      <c r="I53" s="8"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
@@ -2251,17 +2434,19 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V53" s="3"/>
+      <c r="W53" s="3"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="8"/>
+      <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
+      <c r="I54" s="8"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
@@ -2274,17 +2459,19 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V54" s="3"/>
+      <c r="W54" s="3"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="8"/>
+      <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
+      <c r="I55" s="8"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
@@ -2297,17 +2484,19 @@
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
       <c r="U55" s="3"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="8"/>
+      <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
+      <c r="I56" s="8"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
@@ -2320,17 +2509,19 @@
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="8"/>
+      <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
+      <c r="I57" s="8"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
@@ -2343,17 +2534,19 @@
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
       <c r="U57" s="3"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V57" s="3"/>
+      <c r="W57" s="3"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="8"/>
+      <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
+      <c r="I58" s="8"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
@@ -2366,17 +2559,19 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V58" s="3"/>
+      <c r="W58" s="3"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="8"/>
+      <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
+      <c r="I59" s="8"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
@@ -2389,17 +2584,19 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
       <c r="U59" s="3"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V59" s="3"/>
+      <c r="W59" s="3"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="8"/>
+      <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
+      <c r="I60" s="8"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
@@ -2412,17 +2609,19 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V60" s="3"/>
+      <c r="W60" s="3"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="8"/>
+      <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
+      <c r="I61" s="8"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
@@ -2435,17 +2634,19 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
       <c r="U61" s="3"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V61" s="3"/>
+      <c r="W61" s="3"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="8"/>
+      <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
+      <c r="I62" s="8"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
@@ -2458,17 +2659,19 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="8"/>
+      <c r="G63" s="3"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
+      <c r="I63" s="8"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
@@ -2481,17 +2684,19 @@
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
       <c r="U63" s="3"/>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="8"/>
+      <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
+      <c r="I64" s="8"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
@@ -2504,17 +2709,19 @@
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
       <c r="U64" s="3"/>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V64" s="3"/>
+      <c r="W64" s="3"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="8"/>
+      <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
+      <c r="I65" s="8"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
@@ -2527,17 +2734,19 @@
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
       <c r="U65" s="3"/>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V65" s="3"/>
+      <c r="W65" s="3"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="8"/>
+      <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
+      <c r="I66" s="8"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
@@ -2550,17 +2759,19 @@
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
       <c r="U66" s="3"/>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V66" s="3"/>
+      <c r="W66" s="3"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
-      <c r="G67" s="8"/>
+      <c r="G67" s="3"/>
       <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
+      <c r="I67" s="8"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
@@ -2573,17 +2784,19 @@
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
       <c r="U67" s="3"/>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="8"/>
+      <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
+      <c r="I68" s="8"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
@@ -2596,17 +2809,19 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
       <c r="U68" s="3"/>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
-      <c r="G69" s="8"/>
+      <c r="G69" s="3"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
+      <c r="I69" s="8"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
@@ -2619,17 +2834,19 @@
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
       <c r="U69" s="3"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V69" s="3"/>
+      <c r="W69" s="3"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="8"/>
+      <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
+      <c r="I70" s="8"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
@@ -2642,17 +2859,19 @@
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
       <c r="U70" s="3"/>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V70" s="3"/>
+      <c r="W70" s="3"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="8"/>
+      <c r="G71" s="3"/>
       <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
+      <c r="I71" s="8"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
@@ -2665,17 +2884,19 @@
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
       <c r="U71" s="3"/>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V71" s="3"/>
+      <c r="W71" s="3"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="8"/>
+      <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
+      <c r="I72" s="8"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
@@ -2688,17 +2909,19 @@
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
       <c r="U72" s="3"/>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V72" s="3"/>
+      <c r="W72" s="3"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="8"/>
+      <c r="G73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
+      <c r="I73" s="8"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
@@ -2711,17 +2934,19 @@
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
       <c r="U73" s="3"/>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V73" s="3"/>
+      <c r="W73" s="3"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="8"/>
+      <c r="G74" s="3"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
+      <c r="I74" s="8"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
@@ -2734,17 +2959,19 @@
       <c r="S74" s="3"/>
       <c r="T74" s="3"/>
       <c r="U74" s="3"/>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V74" s="3"/>
+      <c r="W74" s="3"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="8"/>
+      <c r="G75" s="3"/>
       <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
+      <c r="I75" s="8"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
@@ -2757,17 +2984,19 @@
       <c r="S75" s="3"/>
       <c r="T75" s="3"/>
       <c r="U75" s="3"/>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V75" s="3"/>
+      <c r="W75" s="3"/>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
-      <c r="G76" s="8"/>
+      <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
+      <c r="I76" s="8"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
@@ -2780,17 +3009,19 @@
       <c r="S76" s="3"/>
       <c r="T76" s="3"/>
       <c r="U76" s="3"/>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V76" s="3"/>
+      <c r="W76" s="3"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="8"/>
+      <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
+      <c r="I77" s="8"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
@@ -2803,17 +3034,19 @@
       <c r="S77" s="3"/>
       <c r="T77" s="3"/>
       <c r="U77" s="3"/>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V77" s="3"/>
+      <c r="W77" s="3"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="8"/>
+      <c r="G78" s="3"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
+      <c r="I78" s="8"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
@@ -2826,17 +3059,19 @@
       <c r="S78" s="3"/>
       <c r="T78" s="3"/>
       <c r="U78" s="3"/>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="8"/>
+      <c r="G79" s="3"/>
       <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
+      <c r="I79" s="8"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
@@ -2849,17 +3084,19 @@
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V79" s="3"/>
+      <c r="W79" s="3"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="8"/>
+      <c r="G80" s="3"/>
       <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
+      <c r="I80" s="8"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
@@ -2872,17 +3109,19 @@
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V80" s="3"/>
+      <c r="W80" s="3"/>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
-      <c r="G81" s="8"/>
+      <c r="G81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
+      <c r="I81" s="8"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
@@ -2895,17 +3134,19 @@
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
       <c r="U81" s="3"/>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V81" s="3"/>
+      <c r="W81" s="3"/>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="8"/>
+      <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
+      <c r="I82" s="8"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
@@ -2918,17 +3159,19 @@
       <c r="S82" s="3"/>
       <c r="T82" s="3"/>
       <c r="U82" s="3"/>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V82" s="3"/>
+      <c r="W82" s="3"/>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
-      <c r="G83" s="8"/>
+      <c r="G83" s="3"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
+      <c r="I83" s="8"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
@@ -2941,17 +3184,19 @@
       <c r="S83" s="3"/>
       <c r="T83" s="3"/>
       <c r="U83" s="3"/>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V83" s="3"/>
+      <c r="W83" s="3"/>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="8"/>
+      <c r="G84" s="3"/>
       <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
+      <c r="I84" s="8"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
@@ -2964,17 +3209,19 @@
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
       <c r="U84" s="3"/>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V84" s="3"/>
+      <c r="W84" s="3"/>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
-      <c r="G85" s="8"/>
+      <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
+      <c r="I85" s="8"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
@@ -2987,17 +3234,19 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
       <c r="U85" s="3"/>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V85" s="3"/>
+      <c r="W85" s="3"/>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="8"/>
+      <c r="G86" s="3"/>
       <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
+      <c r="I86" s="8"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
@@ -3010,17 +3259,19 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
       <c r="U86" s="3"/>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V86" s="3"/>
+      <c r="W86" s="3"/>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
-      <c r="G87" s="8"/>
+      <c r="G87" s="3"/>
       <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
+      <c r="I87" s="8"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
@@ -3033,17 +3284,19 @@
       <c r="S87" s="3"/>
       <c r="T87" s="3"/>
       <c r="U87" s="3"/>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V87" s="3"/>
+      <c r="W87" s="3"/>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="8"/>
+      <c r="G88" s="3"/>
       <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
+      <c r="I88" s="8"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
@@ -3056,17 +3309,19 @@
       <c r="S88" s="3"/>
       <c r="T88" s="3"/>
       <c r="U88" s="3"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V88" s="3"/>
+      <c r="W88" s="3"/>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="8"/>
+      <c r="G89" s="3"/>
       <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
+      <c r="I89" s="8"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
@@ -3079,17 +3334,19 @@
       <c r="S89" s="3"/>
       <c r="T89" s="3"/>
       <c r="U89" s="3"/>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V89" s="3"/>
+      <c r="W89" s="3"/>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="8"/>
+      <c r="G90" s="3"/>
       <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
+      <c r="I90" s="8"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
@@ -3102,17 +3359,19 @@
       <c r="S90" s="3"/>
       <c r="T90" s="3"/>
       <c r="U90" s="3"/>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="8"/>
+      <c r="G91" s="3"/>
       <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
+      <c r="I91" s="8"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
@@ -3125,17 +3384,19 @@
       <c r="S91" s="3"/>
       <c r="T91" s="3"/>
       <c r="U91" s="3"/>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="8"/>
+      <c r="G92" s="3"/>
       <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
+      <c r="I92" s="8"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
@@ -3148,17 +3409,19 @@
       <c r="S92" s="3"/>
       <c r="T92" s="3"/>
       <c r="U92" s="3"/>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="8"/>
+      <c r="G93" s="3"/>
       <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
+      <c r="I93" s="8"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
@@ -3171,17 +3434,19 @@
       <c r="S93" s="3"/>
       <c r="T93" s="3"/>
       <c r="U93" s="3"/>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V93" s="3"/>
+      <c r="W93" s="3"/>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="8"/>
+      <c r="G94" s="3"/>
       <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
+      <c r="I94" s="8"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
@@ -3194,17 +3459,19 @@
       <c r="S94" s="3"/>
       <c r="T94" s="3"/>
       <c r="U94" s="3"/>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V94" s="3"/>
+      <c r="W94" s="3"/>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="8"/>
+      <c r="G95" s="3"/>
       <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
+      <c r="I95" s="8"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
@@ -3217,17 +3484,19 @@
       <c r="S95" s="3"/>
       <c r="T95" s="3"/>
       <c r="U95" s="3"/>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V95" s="3"/>
+      <c r="W95" s="3"/>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="8"/>
+      <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
+      <c r="I96" s="8"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
@@ -3240,17 +3509,19 @@
       <c r="S96" s="3"/>
       <c r="T96" s="3"/>
       <c r="U96" s="3"/>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V96" s="3"/>
+      <c r="W96" s="3"/>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
-      <c r="G97" s="8"/>
+      <c r="G97" s="3"/>
       <c r="H97" s="3"/>
-      <c r="I97" s="3"/>
+      <c r="I97" s="8"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
@@ -3263,17 +3534,19 @@
       <c r="S97" s="3"/>
       <c r="T97" s="3"/>
       <c r="U97" s="3"/>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V97" s="3"/>
+      <c r="W97" s="3"/>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="8"/>
+      <c r="G98" s="3"/>
       <c r="H98" s="3"/>
-      <c r="I98" s="3"/>
+      <c r="I98" s="8"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
@@ -3286,17 +3559,19 @@
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V98" s="3"/>
+      <c r="W98" s="3"/>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
-      <c r="G99" s="8"/>
+      <c r="G99" s="3"/>
       <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
+      <c r="I99" s="8"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
@@ -3309,17 +3584,19 @@
       <c r="S99" s="3"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V99" s="3"/>
+      <c r="W99" s="3"/>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
-      <c r="G100" s="8"/>
+      <c r="G100" s="3"/>
       <c r="H100" s="3"/>
-      <c r="I100" s="3"/>
+      <c r="I100" s="8"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
@@ -3332,17 +3609,19 @@
       <c r="S100" s="3"/>
       <c r="T100" s="3"/>
       <c r="U100" s="3"/>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V100" s="3"/>
+      <c r="W100" s="3"/>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
-      <c r="G101" s="8"/>
+      <c r="G101" s="3"/>
       <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
+      <c r="I101" s="8"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
@@ -3355,17 +3634,19 @@
       <c r="S101" s="3"/>
       <c r="T101" s="3"/>
       <c r="U101" s="3"/>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V101" s="3"/>
+      <c r="W101" s="3"/>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
-      <c r="G102" s="8"/>
+      <c r="G102" s="3"/>
       <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
+      <c r="I102" s="8"/>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
@@ -3378,49 +3659,472 @@
       <c r="S102" s="3"/>
       <c r="T102" s="3"/>
       <c r="U102" s="3"/>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="9"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
-      <c r="J103" s="4"/>
-      <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
-      <c r="M103" s="4"/>
-      <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
-      <c r="Q103" s="4"/>
-      <c r="R103" s="4"/>
-      <c r="S103" s="4"/>
-      <c r="T103" s="4"/>
-      <c r="U103" s="4"/>
+      <c r="V102" s="3"/>
+      <c r="W102" s="3"/>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="8"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+      <c r="M103" s="3"/>
+      <c r="N103" s="3"/>
+      <c r="O103" s="3"/>
+      <c r="P103" s="3"/>
+      <c r="Q103" s="3"/>
+      <c r="R103" s="3"/>
+      <c r="S103" s="3"/>
+      <c r="T103" s="3"/>
+      <c r="U103" s="3"/>
+      <c r="V103" s="3"/>
+      <c r="W103" s="3"/>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="8"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="3"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="3"/>
+      <c r="P104" s="3"/>
+      <c r="Q104" s="3"/>
+      <c r="R104" s="3"/>
+      <c r="S104" s="3"/>
+      <c r="T104" s="3"/>
+      <c r="U104" s="3"/>
+      <c r="V104" s="3"/>
+      <c r="W104" s="3"/>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+      <c r="M105" s="3"/>
+      <c r="N105" s="3"/>
+      <c r="O105" s="3"/>
+      <c r="P105" s="3"/>
+      <c r="Q105" s="3"/>
+      <c r="R105" s="3"/>
+      <c r="S105" s="3"/>
+      <c r="T105" s="3"/>
+      <c r="U105" s="3"/>
+      <c r="V105" s="3"/>
+      <c r="W105" s="3"/>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="8"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3"/>
+      <c r="P106" s="3"/>
+      <c r="Q106" s="3"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="3"/>
+      <c r="T106" s="3"/>
+      <c r="U106" s="3"/>
+      <c r="V106" s="3"/>
+      <c r="W106" s="3"/>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A107" s="3"/>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="8"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+      <c r="M107" s="3"/>
+      <c r="N107" s="3"/>
+      <c r="O107" s="3"/>
+      <c r="P107" s="3"/>
+      <c r="Q107" s="3"/>
+      <c r="R107" s="3"/>
+      <c r="S107" s="3"/>
+      <c r="T107" s="3"/>
+      <c r="U107" s="3"/>
+      <c r="V107" s="3"/>
+      <c r="W107" s="3"/>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A108" s="3"/>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="8"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="3"/>
+      <c r="T108" s="3"/>
+      <c r="U108" s="3"/>
+      <c r="V108" s="3"/>
+      <c r="W108" s="3"/>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="8"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
+      <c r="O109" s="3"/>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="3"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="3"/>
+      <c r="T109" s="3"/>
+      <c r="U109" s="3"/>
+      <c r="V109" s="3"/>
+      <c r="W109" s="3"/>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A110" s="3"/>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+      <c r="I110" s="8"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="3"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="3"/>
+      <c r="P110" s="3"/>
+      <c r="Q110" s="3"/>
+      <c r="R110" s="3"/>
+      <c r="S110" s="3"/>
+      <c r="T110" s="3"/>
+      <c r="U110" s="3"/>
+      <c r="V110" s="3"/>
+      <c r="W110" s="3"/>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A111" s="3"/>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="8"/>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="3"/>
+      <c r="M111" s="3"/>
+      <c r="N111" s="3"/>
+      <c r="O111" s="3"/>
+      <c r="P111" s="3"/>
+      <c r="Q111" s="3"/>
+      <c r="R111" s="3"/>
+      <c r="S111" s="3"/>
+      <c r="T111" s="3"/>
+      <c r="U111" s="3"/>
+      <c r="V111" s="3"/>
+      <c r="W111" s="3"/>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A112" s="3"/>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="8"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
+      <c r="M112" s="3"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="3"/>
+      <c r="P112" s="3"/>
+      <c r="Q112" s="3"/>
+      <c r="R112" s="3"/>
+      <c r="S112" s="3"/>
+      <c r="T112" s="3"/>
+      <c r="U112" s="3"/>
+      <c r="V112" s="3"/>
+      <c r="W112" s="3"/>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+      <c r="I113" s="8"/>
+      <c r="J113" s="3"/>
+      <c r="K113" s="3"/>
+      <c r="L113" s="3"/>
+      <c r="M113" s="3"/>
+      <c r="N113" s="3"/>
+      <c r="O113" s="3"/>
+      <c r="P113" s="3"/>
+      <c r="Q113" s="3"/>
+      <c r="R113" s="3"/>
+      <c r="S113" s="3"/>
+      <c r="T113" s="3"/>
+      <c r="U113" s="3"/>
+      <c r="V113" s="3"/>
+      <c r="W113" s="3"/>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A114" s="3"/>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="3"/>
+      <c r="I114" s="8"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="3"/>
+      <c r="M114" s="3"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="3"/>
+      <c r="P114" s="3"/>
+      <c r="Q114" s="3"/>
+      <c r="R114" s="3"/>
+      <c r="S114" s="3"/>
+      <c r="T114" s="3"/>
+      <c r="U114" s="3"/>
+      <c r="V114" s="3"/>
+      <c r="W114" s="3"/>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A115" s="3"/>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="8"/>
+      <c r="J115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="3"/>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3"/>
+      <c r="O115" s="3"/>
+      <c r="P115" s="3"/>
+      <c r="Q115" s="3"/>
+      <c r="R115" s="3"/>
+      <c r="S115" s="3"/>
+      <c r="T115" s="3"/>
+      <c r="U115" s="3"/>
+      <c r="V115" s="3"/>
+      <c r="W115" s="3"/>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A116" s="3"/>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
+      <c r="I116" s="8"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="3"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="3"/>
+      <c r="P116" s="3"/>
+      <c r="Q116" s="3"/>
+      <c r="R116" s="3"/>
+      <c r="S116" s="3"/>
+      <c r="T116" s="3"/>
+      <c r="U116" s="3"/>
+      <c r="V116" s="3"/>
+      <c r="W116" s="3"/>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A117" s="3"/>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+      <c r="I117" s="8"/>
+      <c r="J117" s="3"/>
+      <c r="K117" s="3"/>
+      <c r="L117" s="3"/>
+      <c r="M117" s="3"/>
+      <c r="N117" s="3"/>
+      <c r="O117" s="3"/>
+      <c r="P117" s="3"/>
+      <c r="Q117" s="3"/>
+      <c r="R117" s="3"/>
+      <c r="S117" s="3"/>
+      <c r="T117" s="3"/>
+      <c r="U117" s="3"/>
+      <c r="V117" s="3"/>
+      <c r="W117" s="3"/>
+    </row>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A118" s="3"/>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="8"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="3"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="3"/>
+      <c r="P118" s="3"/>
+      <c r="Q118" s="3"/>
+      <c r="R118" s="3"/>
+      <c r="S118" s="3"/>
+      <c r="T118" s="3"/>
+      <c r="U118" s="3"/>
+      <c r="V118" s="3"/>
+      <c r="W118" s="3"/>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A119" s="3"/>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3"/>
+      <c r="I119" s="8"/>
+      <c r="J119" s="3"/>
+      <c r="K119" s="3"/>
+      <c r="L119" s="3"/>
+      <c r="M119" s="3"/>
+      <c r="N119" s="3"/>
+      <c r="O119" s="3"/>
+      <c r="P119" s="3"/>
+      <c r="Q119" s="3"/>
+      <c r="R119" s="3"/>
+      <c r="S119" s="3"/>
+      <c r="T119" s="3"/>
+      <c r="U119" s="3"/>
+      <c r="V119" s="3"/>
+      <c r="W119" s="3"/>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
+      <c r="L120" s="4"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="4"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="4"/>
+      <c r="R120" s="4"/>
+      <c r="S120" s="4"/>
+      <c r="T120" s="4"/>
+      <c r="U120" s="4"/>
+      <c r="V120" s="4"/>
+      <c r="W120" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="H10:Q10"/>
-    <mergeCell ref="R10:U10"/>
-    <mergeCell ref="H1:U1"/>
+  <mergeCells count="5">
+    <mergeCell ref="J10:S10"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="J1:W1"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e0352403-46d5-4404-bdbc-1f0a648539c7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100480609C1FC1C67448972BF6E5C213C9B" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d8a27d9f643bca640a830f63900ba095">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e0352403-46d5-4404-bdbc-1f0a648539c7" xmlns:ns4="feae19be-fc38-4e70-8c6b-d8d29387d881" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4dd7b5054fe6e24c3fe359ff6c54fc9b" ns3:_="" ns4:_="">
     <xsd:import namespace="e0352403-46d5-4404-bdbc-1f0a648539c7"/>
@@ -3667,6 +4371,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e0352403-46d5-4404-bdbc-1f0a648539c7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3677,23 +4389,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA175FFD-CB56-494C-9EA7-2E291C339341}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e0352403-46d5-4404-bdbc-1f0a648539c7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="feae19be-fc38-4e70-8c6b-d8d29387d881"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{265F0BE7-781C-40F7-87F8-6CB58D378A12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3712,6 +4407,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA175FFD-CB56-494C-9EA7-2E291C339341}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e0352403-46d5-4404-bdbc-1f0a648539c7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="feae19be-fc38-4e70-8c6b-d8d29387d881"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD43763C-740C-46F8-BCA2-7E25E668CF75}">
   <ds:schemaRefs>

</xml_diff>